<commit_message>
Updated GUI and added functions to return movies based on actor and return actor based on movies
</commit_message>
<xml_diff>
--- a/testData/testMovies.xlsx
+++ b/testData/testMovies.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MengSpring\data-692\ENSF692-Project\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87D0BC1F-A0C8-4789-8D7F-FC93B03726CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF3E174-2D79-49C1-98EC-D351F5B4F439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{A39412BA-4797-498C-B925-F034EBBE45B6}"/>
+    <workbookView xWindow="3420" yWindow="2710" windowWidth="19200" windowHeight="11170" xr2:uid="{A39412BA-4797-498C-B925-F034EBBE45B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -430,7 +430,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB866DCE-E701-473F-A9E2-A21458EE9FFC}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>

</xml_diff>